<commit_message>
Hiển thị danh sách item, item hiển thị ảnh, tên cơ bản. Những item có thể trable, của nhiều steamid khác nhau.
</commit_message>
<xml_diff>
--- a/Requirement SteamTrade.xlsx
+++ b/Requirement SteamTrade.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="80">
   <si>
     <t>Tổng quan</t>
   </si>
@@ -257,6 +257,12 @@
   </si>
   <si>
     <t>Thiết kế cơ sở dữ liệu, Code cấu trúc tổng thể và các nghiệp vụ cơ bản</t>
+  </si>
+  <si>
+    <t>Còn giá</t>
+  </si>
+  <si>
+    <t>Liên kết lấy giá tham khảo trên analyst</t>
   </si>
 </sst>
 </file>
@@ -348,7 +354,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -399,6 +405,9 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -407,6 +416,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -716,7 +728,7 @@
   <dimension ref="B1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -728,22 +740,22 @@
     <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.140625" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" style="18" customWidth="1"/>
     <col min="10" max="10" width="36.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:10" ht="21" x14ac:dyDescent="0.25">
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
     </row>
     <row r="2" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B2" s="13" t="s">
@@ -797,7 +809,9 @@
         <f>G3+F3-1</f>
         <v>42815</v>
       </c>
-      <c r="I3" s="7"/>
+      <c r="I3" s="22">
+        <v>0.3</v>
+      </c>
       <c r="J3" s="11"/>
     </row>
     <row r="4" spans="2:10" ht="105" x14ac:dyDescent="0.25">
@@ -824,7 +838,7 @@
         <f t="shared" ref="H4:H7" si="0">G4+F4-1</f>
         <v>42816</v>
       </c>
-      <c r="I4" s="7"/>
+      <c r="I4" s="6"/>
       <c r="J4" s="12" t="s">
         <v>75</v>
       </c>
@@ -853,8 +867,12 @@
         <f t="shared" si="0"/>
         <v>42818</v>
       </c>
-      <c r="I5" s="7"/>
-      <c r="J5" s="11"/>
+      <c r="I5" s="22">
+        <v>0.8</v>
+      </c>
+      <c r="J5" s="11" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" s="7">
@@ -880,8 +898,12 @@
         <f t="shared" si="0"/>
         <v>42822</v>
       </c>
-      <c r="I6" s="7"/>
-      <c r="J6" s="11"/>
+      <c r="I6" s="22">
+        <v>0.8</v>
+      </c>
+      <c r="J6" s="11" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="7" spans="2:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B7" s="7">
@@ -907,7 +929,7 @@
         <f t="shared" si="0"/>
         <v>42825</v>
       </c>
-      <c r="I7" s="7"/>
+      <c r="I7" s="6"/>
       <c r="J7" s="11"/>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
@@ -954,13 +976,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
     </row>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -1046,13 +1068,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
     </row>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -1137,13 +1159,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
     </row>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -1214,13 +1236,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
     </row>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -1402,7 +1424,7 @@
       <c r="C11" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="19" t="s">
+      <c r="D11" s="20" t="s">
         <v>15</v>
       </c>
       <c r="E11" t="s">
@@ -1413,7 +1435,7 @@
       <c r="C12" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="19"/>
+      <c r="D12" s="20"/>
       <c r="E12" t="s">
         <v>17</v>
       </c>
@@ -1422,7 +1444,7 @@
       <c r="C13" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="19"/>
+      <c r="D13" s="20"/>
       <c r="E13" t="s">
         <v>19</v>
       </c>

</xml_diff>